<commit_message>
* new battle doing...
</commit_message>
<xml_diff>
--- a/plan/excel/creature_team_怪物队伍表.xlsx
+++ b/plan/excel/creature_team_怪物队伍表.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
   <si>
     <t>number</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -106,18 +106,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>上位</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>中位</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>下位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>desc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -150,37 +138,82 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>top#id_lv</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>mid#id_lv</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>10001_1</t>
   </si>
   <si>
+    <t>10003_1</t>
+  </si>
+  <si>
+    <t>10004_1</t>
+  </si>
+  <si>
+    <t>10005_1</t>
+  </si>
+  <si>
+    <t>10006_1</t>
+  </si>
+  <si>
+    <t>jl</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>左先锋</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>右先锋</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>主将</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>左辅助</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>右辅助</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>l_pioneer#id_lv</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_pioneer#id_lv</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>commander#id_lv</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>l_guarder#id_lv</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_guarder#id_lv</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
     <t>10002_1</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>10003_1</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>10004_1</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>10005_1</t>
-  </si>
-  <si>
-    <t>10006_1</t>
-  </si>
-  <si>
-    <t>btm#id_lv</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>jl</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>10001_1</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -565,22 +598,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5:C8"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="11.25" customWidth="1"/>
-    <col min="3" max="3" width="15.625" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="3" max="7" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -588,16 +619,22 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -605,7 +642,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>4</v>
@@ -613,25 +650,37 @@
       <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+        <v>29</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -639,107 +688,149 @@
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="D5" s="3" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="D6" s="3" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+        <v>17</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+        <v>18</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+        <v>19</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>